<commit_message>
APW-2 Automate Login Functionality [Test Cases attached]
</commit_message>
<xml_diff>
--- a/Test cases_AutomationPractice.xlsx
+++ b/Test cases_AutomationPractice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software testing\Automation Testing Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC84EE78-0AE4-42C0-BDD8-B40B8D963FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BA0555-3746-4867-B72A-D2FF6C9F5452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D78CB506-DBC1-4A8C-BE4B-E63580455937}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D78CB506-DBC1-4A8C-BE4B-E63580455937}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="99">
   <si>
     <t>Project Name (Client Name)</t>
   </si>
@@ -345,6 +345,54 @@
   </si>
   <si>
     <t>Nikunj Radadiya</t>
+  </si>
+  <si>
+    <t>APW_02_002</t>
+  </si>
+  <si>
+    <t>Validate navigating to "Sign In" (Registration) page from website header</t>
+  </si>
+  <si>
+    <t>Open website (http://automationpractice.com/index.php/) from any supported browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open website 
+2. Navigate to "Sign in" link on website header at right top side
+</t>
+  </si>
+  <si>
+    <t>1. Website should navigate user to "Sign in" page</t>
+  </si>
+  <si>
+    <t>Validate Log in by providing valid mandatory details for "Already Registered" tab</t>
+  </si>
+  <si>
+    <t>Open website (http://automationpractice.com/index.php from any supported browser</t>
+  </si>
+  <si>
+    <t>1. Open website 
+2. Navigate to "Sign in" link on website header at right top side
+3. Fill in Test data "Email Address" and "Password" in "Already Registered" fields
+4. Clock on "Sign in" button</t>
+  </si>
+  <si>
+    <t>Email Address: QATestingtrials@gmail.com
+Password: QATesting@123</t>
+  </si>
+  <si>
+    <t>1. User should be able to Login to the page</t>
+  </si>
+  <si>
+    <t>Validate Log in by providing invalid mandatory details for "Already Registered" tab</t>
+  </si>
+  <si>
+    <t>Email Address: xyz@gmail.com
+Password: xyz@123</t>
+  </si>
+  <si>
+    <t>1. User should not be able to Login to the page
+2. There should be an error message "There is 1 error
+1. Authentication failed."</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878562F5-1099-4192-9D96-47AC99D423A3}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
@@ -1268,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D7671E-6C36-4B24-AE73-056DD7B7D46A}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1333,19 +1381,19 @@
         <v>77</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>35</v>
@@ -1359,27 +1407,27 @@
       <c r="K2" s="26"/>
       <c r="L2" s="27"/>
     </row>
-    <row r="3" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="28" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>35</v>
@@ -1393,7 +1441,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="27"/>
     </row>
-    <row r="4" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="28" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -1401,19 +1449,19 @@
         <v>77</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>35</v>
@@ -1427,295 +1475,8 @@
       <c r="K4" s="23"/>
       <c r="L4" s="27"/>
     </row>
-    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="27"/>
-    </row>
-    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="27"/>
-    </row>
-    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="23"/>
-    </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="23"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
APW-2 Automate Login Functionality
</commit_message>
<xml_diff>
--- a/Test cases_AutomationPractice.xlsx
+++ b/Test cases_AutomationPractice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software testing\Automation Testing Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BA0555-3746-4867-B72A-D2FF6C9F5452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D664A4-B12C-44DD-BDCA-06B8B84C2689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D78CB506-DBC1-4A8C-BE4B-E63580455937}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="99">
   <si>
     <t>Project Name (Client Name)</t>
   </si>
@@ -1316,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D7671E-6C36-4B24-AE73-056DD7B7D46A}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="28" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>76</v>
       </c>
@@ -1474,6 +1474,40 @@
       </c>
       <c r="K4" s="23"/>
       <c r="L4" s="27"/>
+    </row>
+    <row r="5" spans="1:12" s="28" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
APW-3 Registration test cases
</commit_message>
<xml_diff>
--- a/Test cases_AutomationPractice.xlsx
+++ b/Test cases_AutomationPractice.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software testing\Automation Testing Trial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\Documents\CentralWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D664A4-B12C-44DD-BDCA-06B8B84C2689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40D72F9-BA2F-4135-923D-D304BD92F1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D78CB506-DBC1-4A8C-BE4B-E63580455937}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D78CB506-DBC1-4A8C-BE4B-E63580455937}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="99">
   <si>
     <t>Project Name (Client Name)</t>
   </si>
@@ -1056,20 +1056,20 @@
       <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="D2" s="34"/>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="14" t="s">
         <v>1</v>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="30" t="s">
         <v>2</v>
@@ -1101,47 +1101,47 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="31"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="31"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="31"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="32"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
   </sheetData>
@@ -1162,16 +1162,16 @@
       <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1193,7 +1193,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1202,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1213,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
@@ -1224,7 +1224,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>74</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>78</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>79</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>80</v>
       </c>
@@ -1318,27 +1318,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D7671E-6C36-4B24-AE73-056DD7B7D46A}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="9" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="9"/>
+    <col min="10" max="10" width="11.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="28" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="28" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>76</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="27"/>
     </row>
-    <row r="3" spans="1:12" s="28" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="28" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>86</v>
       </c>
@@ -1441,7 +1441,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="27"/>
     </row>
-    <row r="4" spans="1:12" s="28" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="28" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="27"/>
     </row>
-    <row r="5" spans="1:12" s="28" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="28" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>41</v>
       </c>
@@ -1520,27 +1520,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63354BE2-89F0-4F1A-AA4D-026E9F9CE840}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="9" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="9"/>
+    <col min="10" max="10" width="11.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>30</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="27"/>
     </row>
-    <row r="3" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="28" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>40</v>
       </c>
@@ -1643,278 +1643,118 @@
       <c r="K3" s="23"/>
       <c r="L3" s="27"/>
     </row>
-    <row r="4" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="4" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="29"/>
       <c r="K4" s="23"/>
       <c r="L4" s="27"/>
     </row>
-    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="29"/>
       <c r="K5" s="23"/>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="29"/>
       <c r="K6" s="23"/>
       <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="29"/>
       <c r="K7" s="23"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="29"/>
       <c r="K8" s="23"/>
       <c r="L8" s="27"/>
     </row>
-    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="29"/>
       <c r="K9" s="23"/>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="10" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="29"/>
       <c r="K10" s="23"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>26</v>
-      </c>
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="23"/>
     </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
@@ -1926,7 +1766,7 @@
       <c r="J12" s="29"/>
       <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -1939,7 +1779,7 @@
       <c r="J13" s="29"/>
       <c r="K13" s="23"/>
     </row>
-    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -1952,7 +1792,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="23"/>
     </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -1980,23 +1820,23 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="9" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="9"/>
+    <col min="10" max="10" width="11.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
@@ -2031,7 +1871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>76</v>
       </c>
@@ -2065,7 +1905,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="27"/>
     </row>
-    <row r="3" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="28" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>40</v>
       </c>
@@ -2099,7 +1939,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="27"/>
     </row>
-    <row r="4" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="28" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -2133,7 +1973,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="27"/>
     </row>
-    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2007,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>43</v>
       </c>
@@ -2201,7 +2041,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>44</v>
       </c>
@@ -2235,7 +2075,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>62</v>
       </c>
@@ -2269,7 +2109,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="27"/>
     </row>
-    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>63</v>
       </c>
@@ -2303,7 +2143,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="28" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>65</v>
       </c>
@@ -2337,7 +2177,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
@@ -2370,7 +2210,7 @@
       </c>
       <c r="K11" s="23"/>
     </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
@@ -2382,7 +2222,7 @@
       <c r="J12" s="29"/>
       <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -2395,7 +2235,7 @@
       <c r="J13" s="29"/>
       <c r="K13" s="23"/>
     </row>
-    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -2408,7 +2248,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="23"/>
     </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -2435,23 +2275,23 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="9" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="9"/>
+    <col min="10" max="10" width="11.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>16</v>
       </c>
@@ -2486,7 +2326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="28" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>76</v>
       </c>
@@ -2520,7 +2360,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="27"/>
     </row>
-    <row r="3" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="28" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>40</v>
       </c>
@@ -2554,7 +2394,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="27"/>
     </row>
-    <row r="4" spans="1:12" s="28" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="28" customFormat="1" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -2588,7 +2428,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="27"/>
     </row>
-    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>42</v>
       </c>
@@ -2622,7 +2462,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="27"/>
     </row>
-    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="28" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>43</v>
       </c>
@@ -2656,7 +2496,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="28" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>44</v>
       </c>
@@ -2690,7 +2530,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="27"/>
     </row>
-    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>62</v>
       </c>
@@ -2724,7 +2564,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="27"/>
     </row>
-    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="28" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>63</v>
       </c>
@@ -2758,7 +2598,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="27"/>
     </row>
-    <row r="10" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="28" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>65</v>
       </c>
@@ -2792,7 +2632,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="27"/>
     </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>71</v>
       </c>
@@ -2825,7 +2665,7 @@
       </c>
       <c r="K11" s="23"/>
     </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
@@ -2837,7 +2677,7 @@
       <c r="J12" s="29"/>
       <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -2850,7 +2690,7 @@
       <c r="J13" s="29"/>
       <c r="K13" s="23"/>
     </row>
-    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -2863,7 +2703,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="23"/>
     </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="28" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>

</xml_diff>